<commit_message>
refactor code, better logic for colonies
</commit_message>
<xml_diff>
--- a/colony_planet_build.xlsx
+++ b/colony_planet_build.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="24">
   <si>
     <t>solar_plant</t>
   </si>
@@ -55,12 +55,6 @@
     <t>RoboticsFactory</t>
   </si>
   <si>
-    <t>research_lab</t>
-  </si>
-  <si>
-    <t>ResearchLab</t>
-  </si>
-  <si>
     <t>shipyard</t>
   </si>
   <si>
@@ -73,34 +67,16 @@
     <t>DeuteriumTank</t>
   </si>
   <si>
-    <t>small_shield_dome</t>
-  </si>
-  <si>
-    <t>SmallShieldDome</t>
-  </si>
-  <si>
-    <t>large_shield_dome</t>
-  </si>
-  <si>
-    <t>LargeShieldDome</t>
+    <t>fusion_reactor</t>
+  </si>
+  <si>
+    <t>FusionReactor</t>
   </si>
   <si>
     <t>missile_silo</t>
   </si>
   <si>
     <t>MissileSilo</t>
-  </si>
-  <si>
-    <t>fusion_reactor</t>
-  </si>
-  <si>
-    <t>FusionReactor</t>
-  </si>
-  <si>
-    <t>computer_technology</t>
-  </si>
-  <si>
-    <t>ComputerTechnology</t>
   </si>
   <si>
     <t>nanite_factory</t>
@@ -151,15 +127,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <right/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -170,16 +149,13 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -195,7 +171,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -214,9 +190,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -565,263 +538,263 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B32" s="2">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B33" s="2">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B34" s="2">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B35" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>17</v>
+        <v>6.0</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="7">
-        <v>7.0</v>
+        <v>2</v>
+      </c>
+      <c r="B36" s="2">
+        <v>8.0</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B37" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>7</v>
+        <v>4.0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="2">
-        <v>8.0</v>
+      <c r="A38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="6">
+        <v>4.0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="2">
+      <c r="A39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="7">
         <v>4.0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="6">
-        <v>4.0</v>
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2">
+        <v>11.0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="6">
-        <v>4.0</v>
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2">
+        <v>7.0</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B42" s="2">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="7">
-        <v>8.0</v>
+      <c r="A43" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="6">
+        <v>3.0</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="B44" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="6">
         <v>9.0</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="6">
-        <v>3.0</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B46" s="6">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="6">
-        <v>9.0</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>5</v>
+      <c r="A47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B48" s="6">
-        <v>11.0</v>
+        <v>14.0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="6">
-        <v>14.0</v>
+        <v>12</v>
+      </c>
+      <c r="B49" s="7">
+        <v>5.0</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B50" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>6</v>
+      <c r="A51" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B51" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>7</v>
+        <v>3.0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B52" s="6">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="8">
-        <v>4.0</v>
+      <c r="A53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="6">
+        <v>13.0</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B54" s="6">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="6">
-        <v>13.0</v>
+      <c r="B55" s="7">
+        <v>14.0</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>3</v>
@@ -829,175 +802,175 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="6">
-        <v>12.0</v>
+        <v>2</v>
+      </c>
+      <c r="B56" s="7">
+        <v>15.0</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B57" s="6">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="6">
-        <v>14.0</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B58" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B59" s="6">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B60" s="6">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B61" s="6">
-        <v>13.0</v>
+      <c r="A61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="7">
+        <v>7.0</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="s">
-        <v>6</v>
+      <c r="A62" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B62" s="6">
-        <v>10.0</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>7</v>
+        <v>5.0</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B63" s="6">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B64" s="6">
-        <v>5.0</v>
+        <v>17.0</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="8">
-        <v>7.0</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>9</v>
+      <c r="A65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="11">
+        <v>9.0</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="8">
+      <c r="A66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="6">
+        <v>17.0</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="9">
         <v>6.0</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>13</v>
+      <c r="C67" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B68" s="6">
-        <v>14.0</v>
+        <v>18.0</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B69" s="6">
-        <v>12.0</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>7</v>
+        <v>15.0</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="6">
-        <v>17.0</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B70" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="8">
-        <v>19.0</v>
+      <c r="B71" s="6">
+        <v>18.0</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>1</v>
@@ -1005,141 +978,141 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="6">
-        <v>15.0</v>
+        <v>12</v>
+      </c>
+      <c r="B72" s="7">
+        <v>7.0</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B73" s="6">
-        <v>13.0</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>7</v>
+        <v>19.0</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="8">
-        <v>21.0</v>
+        <v>4</v>
+      </c>
+      <c r="B74" s="6">
+        <v>17.0</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B75" s="6">
         <v>5.0</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B76" s="11">
+        <v>11.0</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B77" s="8">
-        <v>6.0</v>
-      </c>
-      <c r="C77" s="3" t="s">
+      <c r="B77" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B78" s="6">
-        <v>6.0</v>
+        <v>18.0</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B79" s="6">
-        <v>14.0</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B79" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="6">
-        <v>19.0</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>3</v>
+      <c r="A80" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="9">
+        <v>9.0</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B81" s="6">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B82" s="6">
-        <v>18.0</v>
+        <v>21.0</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="6">
-        <v>20.0</v>
+        <v>4</v>
+      </c>
+      <c r="B83" s="7">
+        <v>19.0</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="7">
         <v>9.0</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -1147,109 +1120,109 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="s">
-        <v>6</v>
+      <c r="A85" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B85" s="6">
-        <v>15.0</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>7</v>
+        <v>9.0</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="6">
-        <v>21.0</v>
+      <c r="A86" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86" s="7">
+        <v>7.0</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="s">
-        <v>4</v>
+      <c r="A87" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B87" s="6">
-        <v>19.0</v>
+        <v>7.0</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B88" s="8">
-        <v>22.0</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B88" s="11">
+        <v>12.0</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B89" s="2">
-        <v>8.0</v>
+        <v>2</v>
+      </c>
+      <c r="B89" s="6">
+        <v>22.0</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B90" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>21</v>
+      <c r="A90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>23</v>
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B92" s="6">
-        <v>22.0</v>
+        <v>14</v>
+      </c>
+      <c r="B92" s="2">
+        <v>8.0</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93" s="6">
-        <v>20.0</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>5</v>
+      <c r="A93" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="8">
+      <c r="B94" s="6">
         <v>23.0</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -1258,297 +1231,297 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B95" s="8">
-        <v>23.0</v>
+        <v>4</v>
+      </c>
+      <c r="B95" s="6">
+        <v>21.0</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B96" s="8">
-        <v>17.0</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B96" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B97" s="8">
-        <v>21.0</v>
+        <v>2</v>
+      </c>
+      <c r="B97" s="6">
+        <v>24.0</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B98" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="8"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="11">
+        <v>13.0</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="9">
         <v>10.0</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="5" t="s">
+      <c r="C101" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B99" s="8">
+      <c r="B102" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="6">
         <v>8.0</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D99" s="9"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B100" s="8">
-        <v>8.0</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="5" t="s">
+      <c r="C103" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="6">
-        <v>9.0</v>
-      </c>
-      <c r="C101" s="3" t="s">
+      <c r="B104" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B102" s="6">
-        <v>24.0</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B103" s="6">
-        <v>22.0</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B104" s="8">
-        <v>24.0</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="F104" s="5"/>
-      <c r="G104" s="8"/>
+      <c r="G104" s="11"/>
       <c r="H104" s="3"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B105" s="8">
-        <v>18.0</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B105" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="6"/>
       <c r="H105" s="3"/>
     </row>
     <row r="106">
-      <c r="A106" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B106" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D106" s="9"/>
+      <c r="A106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="6">
+        <v>25.0</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D106" s="8"/>
     </row>
     <row r="107">
-      <c r="A107" s="5" t="s">
-        <v>10</v>
+      <c r="A107" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B107" s="6">
-        <v>9.0</v>
+        <v>25.0</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="D107" s="8"/>
     </row>
     <row r="108">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B108" s="12">
-        <v>8.0</v>
-      </c>
-      <c r="C108" s="3" t="s">
+      <c r="B108" s="9">
+        <v>11.0</v>
+      </c>
+      <c r="C108" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="5" t="s">
-        <v>8</v>
+      <c r="A109" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B109" s="6">
-        <v>10.0</v>
+        <v>23.0</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B110" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="B110" s="11">
+        <v>15.0</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="6">
-        <v>25.0</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>3</v>
+      <c r="A111" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B111" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B112" s="8">
-        <v>25.0</v>
+        <v>2</v>
+      </c>
+      <c r="B112" s="6">
+        <v>26.0</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B113" s="6">
-        <v>23.0</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B113" s="11">
+        <v>16.0</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B114" s="13">
-        <v>9.0</v>
-      </c>
-      <c r="C114" s="11" t="s">
-        <v>27</v>
+      <c r="A114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="11">
+        <v>17.0</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B115" s="6">
-        <v>21.0</v>
+      <c r="B115" s="11">
+        <v>19.0</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="5" t="s">
-        <v>28</v>
+      <c r="A116" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B116" s="6">
-        <v>10.0</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>29</v>
+        <v>26.0</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B117" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="C117" s="11" t="s">
-        <v>31</v>
+      <c r="A117" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117" s="6">
+        <v>23.0</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="6">
-        <v>26.0</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>3</v>
+      <c r="A118" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B119" s="6">
-        <v>26.0</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B119" s="11">
+        <v>20.0</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B120" s="6">
-        <v>23.0</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B120" s="11">
+        <v>21.0</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="121">
@@ -1563,15 +1536,267 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B122" s="13">
+      <c r="A122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="6">
+        <v>27.0</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="6">
+        <v>27.0</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B124" s="9">
         <v>13.0</v>
       </c>
-      <c r="C122" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="C124" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129" s="6">
+        <v>26.0</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B130" s="6">
+        <v>25.0</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131" s="6">
+        <v>27.0</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B133" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="C133" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" s="6">
+        <v>31.0</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="6">
+        <v>26.0</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" s="6">
+        <v>27.0</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="6">
+        <v>32.0</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B140" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="C140" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B141" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" s="6">
+        <v>29.0</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" s="6">
+        <v>33.0</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="10"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="8"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>